<commit_message>
Small updates on the index
</commit_message>
<xml_diff>
--- a/Indice WebVOWL.xlsx
+++ b/Indice WebVOWL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Ambiente de Trabalho\Tese\Projetos\fic.a\fic.a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269AAD65-660C-482F-BC9F-CDC2D23DCD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A443F839-3ED8-4A66-971F-5CD91F20D622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F8F91CF9-9E32-4AFD-8FEC-19AA0A4677BD}"/>
   </bookViews>
@@ -746,7 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -817,9 +817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -828,9 +825,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1238,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68930799-3BF4-4B71-946F-38AD65422F3A}">
   <dimension ref="B3:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="83" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,7 +1267,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="36">
+      <c r="B4" s="34">
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1285,7 +1279,7 @@
       <c r="G4" s="16"/>
     </row>
     <row r="5" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="36">
+      <c r="B5" s="34">
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -1297,7 +1291,7 @@
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="40">
+      <c r="B6" s="38">
         <v>5</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1309,13 +1303,13 @@
       <c r="E6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="25"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="49"/>
+      <c r="D7" s="47"/>
       <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1323,9 +1317,9 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="49"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1333,9 +1327,9 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="49"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1343,9 +1337,9 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="49"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1353,9 +1347,9 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="38"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="49"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1363,9 +1357,9 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="38"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="49"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="5" t="s">
         <v>45</v>
       </c>
@@ -1373,9 +1367,9 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="49"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="5" t="s">
         <v>46</v>
       </c>
@@ -1383,9 +1377,9 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="38"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="49"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
@@ -1393,9 +1387,9 @@
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="38"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="49"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="1" t="s">
         <v>48</v>
       </c>
@@ -1403,9 +1397,9 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="49"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
@@ -1413,9 +1407,9 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="49"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1423,9 +1417,9 @@
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="38"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="49"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1433,37 +1427,37 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="39"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="52" t="s">
+      <c r="D19" s="48"/>
+      <c r="E19" s="50" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="46">
+      <c r="B20" s="44">
         <v>6</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="46"/>
     </row>
     <row r="21" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="37">
+      <c r="B21" s="35">
         <v>7</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="33" t="s">
         <v>66</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -1473,7 +1467,7 @@
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40">
+      <c r="B22" s="38">
         <v>8</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1486,10 +1480,10 @@
       <c r="F22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="29"/>
     </row>
     <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="38"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="5" t="s">
@@ -1501,10 +1495,10 @@
       <c r="G23" s="17"/>
     </row>
     <row r="24" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="39"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="25" t="s">
         <v>54</v>
       </c>
       <c r="F24" s="12" t="s">
@@ -1513,7 +1507,7 @@
       <c r="G24" s="19"/>
     </row>
     <row r="25" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="40">
+      <c r="B25" s="38">
         <v>9</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -1529,17 +1523,17 @@
       <c r="G25" s="24"/>
     </row>
     <row r="26" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="39"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="2:7" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="37">
+      <c r="B27" s="35">
         <v>10</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -1549,11 +1543,11 @@
         <v>57</v>
       </c>
       <c r="E27" s="13"/>
-      <c r="F27" s="30"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="37">
+      <c r="B28" s="35">
         <v>13</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1565,7 +1559,7 @@
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="37">
+      <c r="B29" s="35">
         <v>14</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1577,7 +1571,7 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="37">
+      <c r="B30" s="35">
         <v>16</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -1589,7 +1583,7 @@
       <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="40">
+      <c r="B31" s="38">
         <v>17</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -1598,66 +1592,66 @@
       <c r="D31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="31"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="30" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="38"/>
+      <c r="B32" s="36"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="17"/>
       <c r="F32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="33"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="38"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="33"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="38"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="17"/>
       <c r="F34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="33"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="38"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="17"/>
       <c r="F35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="33"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="39"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="29" t="s">
+      <c r="F36" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="34"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="37">
+      <c r="B37" s="35">
         <v>18</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -1666,14 +1660,14 @@
       <c r="D37" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="43" t="s">
+      <c r="E37" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="37">
+      <c r="B38" s="35">
         <v>19</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -1682,14 +1676,14 @@
       <c r="D38" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="41" t="s">
         <v>26</v>
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="40">
+      <c r="B39" s="38">
         <v>20</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -1701,11 +1695,11 @@
       <c r="E39" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
     </row>
     <row r="40" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="38"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="1" t="s">
@@ -1715,7 +1709,7 @@
       <c r="G40" s="17"/>
     </row>
     <row r="41" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="38"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="1" t="s">
@@ -1725,7 +1719,7 @@
       <c r="G41" s="17"/>
     </row>
     <row r="42" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="39"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10" t="s">
@@ -1735,31 +1729,31 @@
       <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="37">
+      <c r="B43" s="35">
         <v>21</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>64</v>
       </c>
       <c r="D43" s="13"/>
-      <c r="E43" s="45"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
     </row>
     <row r="44" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="37">
+      <c r="B44" s="35">
         <v>22</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D44" s="13"/>
-      <c r="E44" s="45"/>
+      <c r="E44" s="43"/>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
     </row>
     <row r="45" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="37">
+      <c r="B45" s="35">
         <v>26</v>
       </c>
       <c r="C45" s="7" t="s">
@@ -1768,14 +1762,14 @@
       <c r="D45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
     </row>
     <row r="46" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="37">
+      <c r="B46" s="35">
         <v>27</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -1791,7 +1785,7 @@
       <c r="G46" s="13"/>
     </row>
     <row r="47" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="37">
+      <c r="B47" s="35">
         <v>28</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -1800,14 +1794,14 @@
       <c r="D47" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="43" t="s">
+      <c r="E47" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
     </row>
     <row r="48" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="37">
+      <c r="B48" s="35">
         <v>29</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -1823,7 +1817,7 @@
       <c r="G48" s="13"/>
     </row>
     <row r="49" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="37">
+      <c r="B49" s="35">
         <v>30</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -1839,7 +1833,7 @@
       <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="37">
+      <c r="B50" s="35">
         <v>31</v>
       </c>
       <c r="C50" s="7" t="s">
@@ -1848,14 +1842,14 @@
       <c r="D50" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="43" t="s">
+      <c r="E50" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
     </row>
     <row r="51" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="37">
+      <c r="B51" s="35">
         <v>32</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -1871,7 +1865,7 @@
       <c r="G51" s="13"/>
     </row>
     <row r="52" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="37">
+      <c r="B52" s="35">
         <v>33</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -1880,14 +1874,14 @@
       <c r="D52" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="43" t="s">
+      <c r="E52" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
     </row>
     <row r="53" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="37">
+      <c r="B53" s="35">
         <v>34</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -1903,7 +1897,7 @@
       <c r="G53" s="13"/>
     </row>
     <row r="54" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="37">
+      <c r="B54" s="35">
         <v>35</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -1917,7 +1911,7 @@
       <c r="G54" s="13"/>
     </row>
     <row r="55" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="40">
+      <c r="B55" s="38">
         <v>36</v>
       </c>
       <c r="C55" s="9" t="s">
@@ -1929,11 +1923,11 @@
       <c r="E55" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
     </row>
     <row r="56" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="38"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="1" t="s">
@@ -1943,7 +1937,7 @@
       <c r="G56" s="17"/>
     </row>
     <row r="57" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="38"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="1" t="s">
@@ -1953,7 +1947,7 @@
       <c r="G57" s="17"/>
     </row>
     <row r="58" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="39"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="12" t="s">
@@ -1963,7 +1957,7 @@
       <c r="G58" s="19"/>
     </row>
     <row r="59" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="37">
+      <c r="B59" s="35">
         <v>37</v>
       </c>
       <c r="C59" s="7" t="s">
@@ -1977,7 +1971,7 @@
       <c r="G59" s="13"/>
     </row>
     <row r="60" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="37">
+      <c r="B60" s="35">
         <v>38</v>
       </c>
       <c r="C60" s="7" t="s">
@@ -1993,7 +1987,7 @@
       <c r="G60" s="13"/>
     </row>
     <row r="61" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="37">
+      <c r="B61" s="35">
         <v>39</v>
       </c>
       <c r="C61" s="7" t="s">
@@ -2002,32 +1996,32 @@
       <c r="D61" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="43" t="s">
+      <c r="E61" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
     </row>
     <row r="62" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="40">
+      <c r="B62" s="38">
         <v>40</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="32" t="s">
+      <c r="D62" s="30" t="s">
         <v>87</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
     </row>
     <row r="63" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="38"/>
+      <c r="B63" s="36"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="33"/>
+      <c r="D63" s="31"/>
       <c r="E63" s="1" t="s">
         <v>74</v>
       </c>
@@ -2035,9 +2029,9 @@
       <c r="G63" s="17"/>
     </row>
     <row r="64" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="38"/>
+      <c r="B64" s="36"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="33"/>
+      <c r="D64" s="31"/>
       <c r="E64" s="1" t="s">
         <v>75</v>
       </c>
@@ -2045,9 +2039,9 @@
       <c r="G64" s="17"/>
     </row>
     <row r="65" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="38"/>
+      <c r="B65" s="36"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="33"/>
+      <c r="D65" s="31"/>
       <c r="E65" s="1" t="s">
         <v>31</v>
       </c>
@@ -2055,9 +2049,9 @@
       <c r="G65" s="17"/>
     </row>
     <row r="66" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="38"/>
+      <c r="B66" s="36"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="33"/>
+      <c r="D66" s="31"/>
       <c r="E66" s="1" t="s">
         <v>76</v>
       </c>
@@ -2065,9 +2059,9 @@
       <c r="G66" s="17"/>
     </row>
     <row r="67" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="38"/>
+      <c r="B67" s="36"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="33"/>
+      <c r="D67" s="31"/>
       <c r="E67" s="1" t="s">
         <v>77</v>
       </c>
@@ -2075,9 +2069,9 @@
       <c r="G67" s="17"/>
     </row>
     <row r="68" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="38"/>
+      <c r="B68" s="36"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="33"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="1" t="s">
         <v>78</v>
       </c>
@@ -2085,9 +2079,9 @@
       <c r="G68" s="17"/>
     </row>
     <row r="69" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="38"/>
+      <c r="B69" s="36"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="33"/>
+      <c r="D69" s="31"/>
       <c r="E69" s="1" t="s">
         <v>79</v>
       </c>
@@ -2095,9 +2089,9 @@
       <c r="G69" s="17"/>
     </row>
     <row r="70" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="38"/>
+      <c r="B70" s="36"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="33"/>
+      <c r="D70" s="31"/>
       <c r="E70" s="1" t="s">
         <v>80</v>
       </c>
@@ -2105,9 +2099,9 @@
       <c r="G70" s="17"/>
     </row>
     <row r="71" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="38"/>
+      <c r="B71" s="36"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="33"/>
+      <c r="D71" s="31"/>
       <c r="E71" s="1" t="s">
         <v>81</v>
       </c>
@@ -2115,9 +2109,9 @@
       <c r="G71" s="17"/>
     </row>
     <row r="72" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="38"/>
+      <c r="B72" s="36"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="33"/>
+      <c r="D72" s="31"/>
       <c r="E72" s="1" t="s">
         <v>82</v>
       </c>
@@ -2125,9 +2119,9 @@
       <c r="G72" s="17"/>
     </row>
     <row r="73" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="38"/>
+      <c r="B73" s="36"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="33"/>
+      <c r="D73" s="31"/>
       <c r="E73" s="1" t="s">
         <v>83</v>
       </c>
@@ -2135,9 +2129,9 @@
       <c r="G73" s="17"/>
     </row>
     <row r="74" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="38"/>
+      <c r="B74" s="36"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="33"/>
+      <c r="D74" s="31"/>
       <c r="E74" s="1" t="s">
         <v>84</v>
       </c>
@@ -2145,9 +2139,9 @@
       <c r="G74" s="17"/>
     </row>
     <row r="75" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="38"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="33"/>
+      <c r="D75" s="31"/>
       <c r="E75" s="1" t="s">
         <v>85</v>
       </c>
@@ -2155,17 +2149,17 @@
       <c r="G75" s="17"/>
     </row>
     <row r="76" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="39"/>
+      <c r="B76" s="37"/>
       <c r="C76" s="11"/>
-      <c r="D76" s="34"/>
-      <c r="E76" s="52" t="s">
+      <c r="D76" s="32"/>
+      <c r="E76" s="50" t="s">
         <v>86</v>
       </c>
       <c r="F76" s="19"/>
       <c r="G76" s="19"/>
     </row>
     <row r="77" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="37">
+      <c r="B77" s="35">
         <v>41</v>
       </c>
       <c r="C77" s="7" t="s">
@@ -2174,14 +2168,14 @@
       <c r="D77" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E77" s="54" t="s">
+      <c r="E77" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
     </row>
     <row r="78" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="40">
+      <c r="B78" s="38">
         <v>42</v>
       </c>
       <c r="C78" s="9" t="s">
@@ -2190,37 +2184,37 @@
       <c r="D78" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E78" s="55" t="s">
+      <c r="E78" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
     </row>
     <row r="79" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="38"/>
+      <c r="B79" s="36"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="53" t="s">
+      <c r="E79" s="51" t="s">
         <v>22</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="17"/>
     </row>
     <row r="80" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="38"/>
+      <c r="B80" s="36"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="53" t="s">
+      <c r="E80" s="51" t="s">
         <v>54</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="17"/>
     </row>
     <row r="81" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="38"/>
+      <c r="B81" s="36"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
-      <c r="E81" s="53" t="s">
+      <c r="E81" s="51" t="s">
         <v>55</v>
       </c>
       <c r="F81" s="17"/>
@@ -2230,27 +2224,27 @@
       </c>
     </row>
     <row r="82" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="38"/>
+      <c r="B82" s="36"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
-      <c r="E82" s="53" t="s">
+      <c r="E82" s="51" t="s">
         <v>70</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="17"/>
     </row>
     <row r="83" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="39"/>
+      <c r="B83" s="37"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
-      <c r="E83" s="56" t="s">
+      <c r="E83" s="54" t="s">
         <v>30</v>
       </c>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
     </row>
     <row r="84" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="37">
+      <c r="B84" s="35">
         <v>43</v>
       </c>
       <c r="C84" s="7" t="s">
@@ -2264,7 +2258,7 @@
       <c r="G84" s="13"/>
     </row>
     <row r="85" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="37">
+      <c r="B85" s="35">
         <v>44</v>
       </c>
       <c r="C85" s="7" t="s">
@@ -2273,14 +2267,14 @@
       <c r="D85" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E85" s="54" t="s">
+      <c r="E85" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
     </row>
     <row r="86" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="37">
+      <c r="B86" s="35">
         <v>45</v>
       </c>
       <c r="C86" s="7" t="s">
@@ -2289,14 +2283,14 @@
       <c r="D86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="54" t="s">
+      <c r="E86" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
     </row>
     <row r="87" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="37">
+      <c r="B87" s="35">
         <v>46</v>
       </c>
       <c r="C87" s="7" t="s">
@@ -2305,14 +2299,14 @@
       <c r="D87" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E87" s="54" t="s">
+      <c r="E87" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
     </row>
     <row r="88" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="37">
+      <c r="B88" s="35">
         <v>47</v>
       </c>
       <c r="C88" s="7" t="s">
@@ -2321,14 +2315,14 @@
       <c r="D88" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E88" s="54" t="s">
+      <c r="E88" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
     </row>
     <row r="89" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="37">
+      <c r="B89" s="35">
         <v>48</v>
       </c>
       <c r="C89" s="7" t="s">
@@ -2337,14 +2331,14 @@
       <c r="D89" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E89" s="54" t="s">
+      <c r="E89" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
     </row>
     <row r="90" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="37">
+      <c r="B90" s="35">
         <v>49</v>
       </c>
       <c r="C90" s="7" t="s">
@@ -2353,14 +2347,14 @@
       <c r="D90" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E90" s="54" t="s">
+      <c r="E90" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F90" s="13"/>
       <c r="G90" s="13"/>
     </row>
     <row r="91" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="37">
+      <c r="B91" s="35">
         <v>50</v>
       </c>
       <c r="C91" s="7" t="s">
@@ -2369,14 +2363,14 @@
       <c r="D91" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E91" s="54" t="s">
+      <c r="E91" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F91" s="13"/>
       <c r="G91" s="13"/>
     </row>
     <row r="92" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="37">
+      <c r="B92" s="35">
         <v>51</v>
       </c>
       <c r="C92" s="7" t="s">
@@ -2385,14 +2379,14 @@
       <c r="D92" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E92" s="54" t="s">
+      <c r="E92" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
     </row>
     <row r="93" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="37">
+      <c r="B93" s="35">
         <v>52</v>
       </c>
       <c r="C93" s="7" t="s">
@@ -2401,14 +2395,14 @@
       <c r="D93" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E93" s="54" t="s">
+      <c r="E93" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
     </row>
     <row r="94" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="37">
+      <c r="B94" s="35">
         <v>53</v>
       </c>
       <c r="C94" s="7" t="s">
@@ -2417,14 +2411,14 @@
       <c r="D94" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E94" s="54" t="s">
+      <c r="E94" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
     </row>
     <row r="95" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="37">
+      <c r="B95" s="35">
         <v>54</v>
       </c>
       <c r="C95" s="7" t="s">
@@ -2433,14 +2427,14 @@
       <c r="D95" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E95" s="54" t="s">
+      <c r="E95" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
     </row>
     <row r="96" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="37">
+      <c r="B96" s="35">
         <v>55</v>
       </c>
       <c r="C96" s="7" t="s">
@@ -2449,14 +2443,14 @@
       <c r="D96" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E96" s="54" t="s">
+      <c r="E96" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
     </row>
     <row r="97" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="37">
+      <c r="B97" s="35">
         <v>56</v>
       </c>
       <c r="C97" s="7" t="s">
@@ -2465,28 +2459,28 @@
       <c r="D97" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E97" s="54" t="s">
+      <c r="E97" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
     </row>
     <row r="98" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="40">
+      <c r="B98" s="38">
         <v>57</v>
       </c>
       <c r="C98" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D98" s="31"/>
+      <c r="D98" s="29"/>
       <c r="E98" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F98" s="31"/>
-      <c r="G98" s="31"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
     </row>
     <row r="99" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="38"/>
+      <c r="B99" s="36"/>
       <c r="C99" s="3"/>
       <c r="D99" s="17"/>
       <c r="E99" s="4" t="s">
@@ -2496,7 +2490,7 @@
       <c r="G99" s="17"/>
     </row>
     <row r="100" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="38"/>
+      <c r="B100" s="36"/>
       <c r="C100" s="3"/>
       <c r="D100" s="17"/>
       <c r="E100" s="4" t="s">
@@ -2506,7 +2500,7 @@
       <c r="G100" s="17"/>
     </row>
     <row r="101" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="38"/>
+      <c r="B101" s="36"/>
       <c r="C101" s="3"/>
       <c r="D101" s="17"/>
       <c r="E101" s="4" t="s">
@@ -2516,7 +2510,7 @@
       <c r="G101" s="17"/>
     </row>
     <row r="102" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="38"/>
+      <c r="B102" s="36"/>
       <c r="C102" s="3"/>
       <c r="D102" s="17"/>
       <c r="E102" s="4" t="s">
@@ -2526,17 +2520,17 @@
       <c r="G102" s="17"/>
     </row>
     <row r="103" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="39"/>
+      <c r="B103" s="37"/>
       <c r="C103" s="11"/>
       <c r="D103" s="19"/>
-      <c r="E103" s="29" t="s">
+      <c r="E103" s="27" t="s">
         <v>63</v>
       </c>
       <c r="F103" s="19"/>
       <c r="G103" s="19"/>
     </row>
     <row r="104" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="41">
+      <c r="B104" s="39">
         <v>58</v>
       </c>
       <c r="C104" s="4" t="s">
@@ -2548,7 +2542,7 @@
       <c r="G104" s="4"/>
     </row>
     <row r="105" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="42">
+      <c r="B105" s="40">
         <v>60</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -2560,7 +2554,7 @@
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="42">
+      <c r="B106" s="40">
         <v>63</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -2572,7 +2566,7 @@
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="42">
+      <c r="B107" s="40">
         <v>64</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -2584,7 +2578,7 @@
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="42">
+      <c r="B108" s="40">
         <v>65</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -2598,7 +2592,7 @@
       <c r="G108" s="1"/>
     </row>
     <row r="109" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="42">
+      <c r="B109" s="40">
         <v>66</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -2610,7 +2604,7 @@
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="42">
+      <c r="B110" s="40">
         <v>67</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -2622,7 +2616,7 @@
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="42">
+      <c r="B111" s="40">
         <v>73</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -2634,7 +2628,7 @@
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="42">
+      <c r="B112" s="40">
         <v>74</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -2646,7 +2640,7 @@
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="42">
+      <c r="B113" s="40">
         <v>75</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -2658,7 +2652,7 @@
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="42">
+      <c r="B114" s="40">
         <v>77</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -2670,7 +2664,7 @@
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="42">
+      <c r="B115" s="40">
         <v>78</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -2682,7 +2676,7 @@
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="42">
+      <c r="B116" s="40">
         <v>79</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -2694,7 +2688,7 @@
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="42">
+      <c r="B117" s="40">
         <v>80</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -2706,7 +2700,7 @@
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="42">
+      <c r="B118" s="40">
         <v>81</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -2718,7 +2712,7 @@
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="42">
+      <c r="B119" s="40">
         <v>82</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -2730,7 +2724,7 @@
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="42">
+      <c r="B120" s="40">
         <v>83</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -2742,7 +2736,7 @@
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="42">
+      <c r="B121" s="40">
         <v>315</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -2754,7 +2748,7 @@
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="42">
+      <c r="B122" s="40">
         <v>316</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -2766,7 +2760,7 @@
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="44">
+      <c r="B123" s="42">
         <v>317</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -2781,10 +2775,10 @@
       <c r="F123" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G123" s="59"/>
+      <c r="G123" s="57"/>
     </row>
     <row r="124" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="44"/>
+      <c r="B124" s="42"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="1" t="s">
@@ -2793,10 +2787,10 @@
       <c r="F124" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G124" s="59"/>
+      <c r="G124" s="57"/>
     </row>
     <row r="125" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="44"/>
+      <c r="B125" s="42"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="1" t="s">
@@ -2805,10 +2799,10 @@
       <c r="F125" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G125" s="59"/>
+      <c r="G125" s="57"/>
     </row>
     <row r="126" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="44"/>
+      <c r="B126" s="42"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
       <c r="E126" s="1" t="s">
@@ -2817,20 +2811,20 @@
       <c r="F126" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G126" s="59"/>
+      <c r="G126" s="57"/>
     </row>
     <row r="127" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="44"/>
+      <c r="B127" s="42"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="57"/>
+      <c r="E127" s="55"/>
       <c r="F127" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G127" s="59"/>
+      <c r="G127" s="57"/>
     </row>
     <row r="128" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="42">
+      <c r="B128" s="40">
         <v>318</v>
       </c>
       <c r="C128" s="1" t="s">
@@ -2842,7 +2836,7 @@
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="42">
+      <c r="B129" s="40">
         <v>319</v>
       </c>
       <c r="C129" s="1" t="s">
@@ -2854,7 +2848,7 @@
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="42">
+      <c r="B130" s="40">
         <v>320</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -2866,12 +2860,12 @@
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B131" s="58"/>
-      <c r="C131" s="58"/>
-      <c r="D131" s="58"/>
-      <c r="E131" s="58"/>
-      <c r="F131" s="58"/>
-      <c r="G131" s="58"/>
+      <c r="B131" s="56"/>
+      <c r="C131" s="56"/>
+      <c r="D131" s="56"/>
+      <c r="E131" s="56"/>
+      <c r="F131" s="56"/>
+      <c r="G131" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="48">

</xml_diff>

<commit_message>
Changes to OWL2VOWL and format files
Changes that would maybe include the individuals in the JSON but it is not changing anything. Some files with the old and desired formats, as weel as the owl2vowl output "owl_desired_format.json"
</commit_message>
<xml_diff>
--- a/Indice WebVOWL.xlsx
+++ b/Indice WebVOWL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Ambiente de Trabalho\Tese\Projetos\fic.a\fic.a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Ambiente de Trabalho\Tese\Projetos\WebVOWL_individual\WebVOWLindividual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A443F839-3ED8-4A66-971F-5CD91F20D622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596DDA11-134F-4DE8-B7A3-34050ED58948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{F8F91CF9-9E32-4AFD-8FEC-19AA0A4677BD}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" xr2:uid="{F8F91CF9-9E32-4AFD-8FEC-19AA0A4677BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>Module</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t xml:space="preserve">Defines some basic graph behaviours (zoom, centering, etc), </t>
+  </si>
+  <si>
+    <t>rdf:type (old InstanceOf)</t>
   </si>
 </sst>
 </file>
@@ -746,7 +749,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -754,9 +757,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -772,147 +772,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1232,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68930799-3BF4-4B71-946F-38AD65422F3A}">
   <dimension ref="B3:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="83" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1247,1302 +1256,1302 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="34">
+      <c r="B4" s="19">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="34">
+      <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="38">
+      <c r="B6" s="40">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="49"/>
     </row>
     <row r="7" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="50"/>
     </row>
     <row r="8" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="5" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="50"/>
     </row>
     <row r="9" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="5" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="36"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="5" t="s">
+      <c r="B10" s="41"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="50"/>
     </row>
     <row r="11" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="36"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="5" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="36"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="5" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="50"/>
     </row>
     <row r="13" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="36"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="5" t="s">
+      <c r="B13" s="41"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="47"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="58"/>
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="47"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="47"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="47"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="36"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="47"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="37"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="50" t="s">
+      <c r="B19" s="42"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="51"/>
     </row>
     <row r="20" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="44">
+      <c r="B20" s="26">
         <v>6</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="46"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="35">
+      <c r="B21" s="20">
         <v>7</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="38">
+      <c r="B22" s="40">
         <v>8</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="43"/>
+      <c r="E22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="29"/>
+      <c r="G22" s="46"/>
     </row>
     <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="36"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="5" t="s">
+      <c r="B23" s="41"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="17"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="37"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="25" t="s">
+      <c r="B24" s="42"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="19"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="38">
+      <c r="B25" s="40">
         <v>9</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="24"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="37"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="25" t="s">
+      <c r="B26" s="42"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="20"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="51"/>
     </row>
     <row r="27" spans="2:7" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="35">
+      <c r="B27" s="20">
         <v>10</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="13"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="35">
+      <c r="B28" s="20">
         <v>13</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="35">
+      <c r="B29" s="20">
         <v>14</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="35">
+      <c r="B30" s="20">
         <v>16</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="38">
+      <c r="B31" s="40">
         <v>17</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="10" t="s">
+      <c r="E31" s="46"/>
+      <c r="F31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="52" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="36"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="4" t="s">
+      <c r="B32" s="41"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="31"/>
+      <c r="G32" s="53"/>
     </row>
     <row r="33" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="36"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="4" t="s">
+      <c r="B33" s="41"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="53"/>
     </row>
     <row r="34" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="36"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="4" t="s">
+      <c r="B34" s="41"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="31"/>
+      <c r="G34" s="53"/>
     </row>
     <row r="35" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="36"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="4" t="s">
+      <c r="B35" s="41"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="31"/>
+      <c r="G35" s="53"/>
     </row>
     <row r="36" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="37"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="27" t="s">
+      <c r="B36" s="42"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="32"/>
+      <c r="G36" s="54"/>
     </row>
     <row r="37" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="35">
+      <c r="B37" s="20">
         <v>18</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="41" t="s">
+      <c r="E37" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="35">
+      <c r="B38" s="20">
         <v>19</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="38">
+      <c r="B39" s="40">
         <v>20</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
     </row>
     <row r="40" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="36"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
       <c r="E40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="36"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
       <c r="E41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
     </row>
     <row r="42" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="37"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10" t="s">
+      <c r="B42" s="42"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
     </row>
     <row r="43" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="35">
+      <c r="B43" s="20">
         <v>21</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="35">
+      <c r="B44" s="20">
         <v>22</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="35">
+      <c r="B45" s="20">
         <v>26</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="41" t="s">
+      <c r="E45" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="35">
+      <c r="B46" s="20">
         <v>27</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="35">
+      <c r="B47" s="20">
         <v>28</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="41" t="s">
+      <c r="E47" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="35">
+      <c r="B48" s="20">
         <v>29</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="35">
+      <c r="B49" s="20">
         <v>30</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="35">
+      <c r="B50" s="20">
         <v>31</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="41" t="s">
+      <c r="E50" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="35">
+      <c r="B51" s="20">
         <v>32</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
     </row>
     <row r="52" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="35">
+      <c r="B52" s="20">
         <v>33</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="41" t="s">
+      <c r="E52" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="35">
+      <c r="B53" s="20">
         <v>34</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
     </row>
     <row r="54" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="35">
+      <c r="B54" s="20">
         <v>35</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7" t="s">
+      <c r="D54" s="6"/>
+      <c r="E54" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
     </row>
     <row r="55" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="38">
+      <c r="B55" s="40">
         <v>36</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
     </row>
     <row r="56" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="36"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
       <c r="E56" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
     </row>
     <row r="57" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="36"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
       <c r="E57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
     </row>
     <row r="58" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="37"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="12" t="s">
+      <c r="B58" s="42"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
     </row>
     <row r="59" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="35">
+      <c r="B59" s="20">
         <v>37</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E59" s="7"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
     </row>
     <row r="60" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="35">
+      <c r="B60" s="20">
         <v>38</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
     </row>
     <row r="61" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="35">
+      <c r="B61" s="20">
         <v>39</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="41" t="s">
+      <c r="E61" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
     </row>
     <row r="62" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="38">
+      <c r="B62" s="40">
         <v>40</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="30" t="s">
+      <c r="D62" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
     </row>
     <row r="63" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="36"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="31"/>
+      <c r="B63" s="41"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="53"/>
       <c r="E63" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
     </row>
     <row r="64" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="36"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="31"/>
+      <c r="B64" s="41"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="53"/>
       <c r="E64" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
     </row>
     <row r="65" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="36"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="31"/>
+      <c r="B65" s="41"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="53"/>
       <c r="E65" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
     </row>
     <row r="66" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="36"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="31"/>
+      <c r="B66" s="41"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="53"/>
       <c r="E66" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
     </row>
     <row r="67" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="36"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="31"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="53"/>
       <c r="E67" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
     </row>
     <row r="68" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="36"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="31"/>
+      <c r="B68" s="41"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="53"/>
       <c r="E68" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
     </row>
     <row r="69" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="36"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="31"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="53"/>
       <c r="E69" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="47"/>
     </row>
     <row r="70" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="36"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="31"/>
+      <c r="B70" s="41"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
     </row>
     <row r="71" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="36"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="31"/>
+      <c r="B71" s="41"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="53"/>
       <c r="E71" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="47"/>
     </row>
     <row r="72" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="36"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="31"/>
+      <c r="B72" s="41"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="53"/>
       <c r="E72" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="47"/>
     </row>
     <row r="73" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="36"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="31"/>
+      <c r="B73" s="41"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="53"/>
       <c r="E73" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
     </row>
     <row r="74" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="36"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="31"/>
+      <c r="B74" s="41"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="53"/>
       <c r="E74" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="47"/>
     </row>
     <row r="75" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="36"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="31"/>
+      <c r="B75" s="41"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="53"/>
       <c r="E75" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
     </row>
     <row r="76" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="37"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="50" t="s">
+      <c r="B76" s="42"/>
+      <c r="C76" s="45"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
     </row>
     <row r="77" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="35">
+      <c r="B77" s="20">
         <v>41</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E77" s="52" t="s">
+      <c r="E77" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
     </row>
     <row r="78" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="38">
+      <c r="B78" s="40">
         <v>42</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="E78" s="53" t="s">
+      <c r="E78" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="46"/>
     </row>
     <row r="79" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="36"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="51" t="s">
+      <c r="B79" s="41"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
+      <c r="F79" s="47"/>
+      <c r="G79" s="47"/>
     </row>
     <row r="80" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="36"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="51" t="s">
+      <c r="B80" s="41"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
+      <c r="F80" s="47"/>
+      <c r="G80" s="47"/>
     </row>
     <row r="81" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="36"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="51" t="s">
+      <c r="B81" s="41"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="47"/>
       <c r="I81" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="82" spans="2:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="36"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="51" t="s">
+      <c r="B82" s="41"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="47"/>
     </row>
     <row r="83" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="37"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="54" t="s">
+      <c r="B83" s="42"/>
+      <c r="C83" s="45"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
+      <c r="F83" s="48"/>
+      <c r="G83" s="48"/>
     </row>
     <row r="84" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="35">
+      <c r="B84" s="20">
         <v>43</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
     </row>
     <row r="85" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="35">
+      <c r="B85" s="20">
         <v>44</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E85" s="52" t="s">
+      <c r="E85" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
     </row>
     <row r="86" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="35">
+      <c r="B86" s="20">
         <v>45</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="52" t="s">
+      <c r="E86" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
     </row>
     <row r="87" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="35">
+      <c r="B87" s="20">
         <v>46</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E87" s="52" t="s">
+      <c r="E87" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
     </row>
     <row r="88" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="35">
+      <c r="B88" s="20">
         <v>47</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E88" s="52" t="s">
+      <c r="E88" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
     </row>
     <row r="89" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="35">
+      <c r="B89" s="20">
         <v>48</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E89" s="52" t="s">
+      <c r="E89" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
     </row>
     <row r="90" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="35">
+      <c r="B90" s="20">
         <v>49</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E90" s="52" t="s">
+      <c r="E90" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
     </row>
     <row r="91" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="35">
+      <c r="B91" s="20">
         <v>50</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="D91" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E91" s="52" t="s">
+      <c r="E91" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
     </row>
     <row r="92" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="35">
+      <c r="B92" s="20">
         <v>51</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E92" s="52" t="s">
+      <c r="E92" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
     </row>
     <row r="93" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="35">
+      <c r="B93" s="20">
         <v>52</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E93" s="52" t="s">
+      <c r="E93" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
     </row>
     <row r="94" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="35">
+      <c r="B94" s="20">
         <v>53</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E94" s="52" t="s">
+      <c r="E94" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
     </row>
     <row r="95" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="35">
+      <c r="B95" s="20">
         <v>54</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E95" s="52" t="s">
+      <c r="E95" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F95" s="13"/>
-      <c r="G95" s="13"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
     </row>
     <row r="96" spans="2:9" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="35">
+      <c r="B96" s="20">
         <v>55</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C96" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E96" s="52" t="s">
+      <c r="E96" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F96" s="13"/>
-      <c r="G96" s="13"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
     </row>
     <row r="97" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="35">
+      <c r="B97" s="20">
         <v>56</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C97" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E97" s="52" t="s">
+      <c r="E97" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
     </row>
     <row r="98" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="38">
+      <c r="B98" s="40">
         <v>57</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D98" s="29"/>
-      <c r="E98" s="10" t="s">
+      <c r="D98" s="46"/>
+      <c r="E98" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F98" s="29"/>
-      <c r="G98" s="29"/>
+      <c r="F98" s="46"/>
+      <c r="G98" s="46"/>
     </row>
     <row r="99" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="36"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="4" t="s">
+      <c r="B99" s="41"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="47"/>
+      <c r="E99" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17"/>
+      <c r="F99" s="47"/>
+      <c r="G99" s="47"/>
     </row>
     <row r="100" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="36"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="4" t="s">
+      <c r="B100" s="41"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="47"/>
+      <c r="E100" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F100" s="17"/>
-      <c r="G100" s="17"/>
+      <c r="F100" s="47"/>
+      <c r="G100" s="47"/>
     </row>
     <row r="101" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="36"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="4" t="s">
+      <c r="B101" s="41"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="47"/>
+      <c r="E101" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F101" s="17"/>
-      <c r="G101" s="17"/>
+      <c r="F101" s="47"/>
+      <c r="G101" s="47"/>
     </row>
     <row r="102" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="36"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="4" t="s">
+      <c r="B102" s="41"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="47"/>
+      <c r="E102" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F102" s="17"/>
-      <c r="G102" s="17"/>
+      <c r="F102" s="47"/>
+      <c r="G102" s="47"/>
     </row>
     <row r="103" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="37"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="27" t="s">
+      <c r="B103" s="42"/>
+      <c r="C103" s="45"/>
+      <c r="D103" s="48"/>
+      <c r="E103" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F103" s="19"/>
-      <c r="G103" s="19"/>
+      <c r="F103" s="48"/>
+      <c r="G103" s="48"/>
     </row>
     <row r="104" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="39">
+      <c r="B104" s="21">
         <v>58</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
     </row>
     <row r="105" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="40">
+      <c r="B105" s="22">
         <v>60</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -2554,7 +2563,7 @@
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="40">
+      <c r="B106" s="22">
         <v>63</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -2566,7 +2575,7 @@
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="40">
+      <c r="B107" s="22">
         <v>64</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -2578,13 +2587,13 @@
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="2:7" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="40">
+      <c r="B108" s="22">
         <v>65</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D108" s="7" t="s">
+      <c r="D108" s="6" t="s">
         <v>89</v>
       </c>
       <c r="E108" s="1"/>
@@ -2592,7 +2601,7 @@
       <c r="G108" s="1"/>
     </row>
     <row r="109" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="40">
+      <c r="B109" s="22">
         <v>66</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -2604,7 +2613,7 @@
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="40">
+      <c r="B110" s="22">
         <v>67</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -2616,7 +2625,7 @@
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="40">
+      <c r="B111" s="22">
         <v>73</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -2628,7 +2637,7 @@
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="40">
+      <c r="B112" s="22">
         <v>74</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -2640,7 +2649,7 @@
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="40">
+      <c r="B113" s="22">
         <v>75</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -2652,7 +2661,7 @@
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="40">
+      <c r="B114" s="22">
         <v>77</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -2664,7 +2673,7 @@
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="40">
+      <c r="B115" s="22">
         <v>78</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -2676,7 +2685,7 @@
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="40">
+      <c r="B116" s="22">
         <v>79</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -2688,7 +2697,7 @@
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="40">
+      <c r="B117" s="22">
         <v>80</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -2700,7 +2709,7 @@
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="40">
+      <c r="B118" s="22">
         <v>81</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -2712,7 +2721,7 @@
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="40">
+      <c r="B119" s="22">
         <v>82</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -2724,7 +2733,7 @@
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="40">
+      <c r="B120" s="22">
         <v>83</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -2736,7 +2745,7 @@
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="40">
+      <c r="B121" s="22">
         <v>315</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -2748,7 +2757,7 @@
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="40">
+      <c r="B122" s="22">
         <v>316</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -2760,13 +2769,13 @@
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="42">
+      <c r="B123" s="37">
         <v>317</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="38" t="s">
         <v>112</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -2775,56 +2784,56 @@
       <c r="F123" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G123" s="57"/>
+      <c r="G123" s="39"/>
     </row>
     <row r="124" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="42"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
+      <c r="B124" s="37"/>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38"/>
       <c r="E124" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G124" s="57"/>
+      <c r="G124" s="39"/>
     </row>
     <row r="125" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="42"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="38"/>
       <c r="E125" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G125" s="57"/>
+      <c r="G125" s="39"/>
     </row>
     <row r="126" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="42"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
+      <c r="B126" s="37"/>
+      <c r="C126" s="38"/>
+      <c r="D126" s="38"/>
       <c r="E126" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G126" s="57"/>
+      <c r="G126" s="39"/>
     </row>
     <row r="127" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="42"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="55"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="35"/>
       <c r="F127" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G127" s="57"/>
+      <c r="G127" s="39"/>
     </row>
     <row r="128" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="40">
+      <c r="B128" s="22">
         <v>318</v>
       </c>
       <c r="C128" s="1" t="s">
@@ -2836,7 +2845,7 @@
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="40">
+      <c r="B129" s="22">
         <v>319</v>
       </c>
       <c r="C129" s="1" t="s">
@@ -2848,7 +2857,7 @@
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="40">
+      <c r="B130" s="22">
         <v>320</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -2860,29 +2869,37 @@
       <c r="G130" s="1"/>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B131" s="56"/>
-      <c r="C131" s="56"/>
-      <c r="D131" s="56"/>
-      <c r="E131" s="56"/>
-      <c r="F131" s="56"/>
-      <c r="G131" s="56"/>
+      <c r="B131" s="24">
+        <v>321</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="36"/>
+      <c r="F131" s="36"/>
+      <c r="G131" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B123:B127"/>
-    <mergeCell ref="C123:C127"/>
-    <mergeCell ref="D123:D127"/>
-    <mergeCell ref="G123:G127"/>
-    <mergeCell ref="B98:B103"/>
-    <mergeCell ref="C98:C103"/>
-    <mergeCell ref="D98:D103"/>
-    <mergeCell ref="F98:F103"/>
-    <mergeCell ref="G98:G103"/>
-    <mergeCell ref="B78:B83"/>
-    <mergeCell ref="C78:C83"/>
-    <mergeCell ref="D78:D83"/>
-    <mergeCell ref="F78:F83"/>
-    <mergeCell ref="G78:G83"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="B6:B19"/>
+    <mergeCell ref="C6:C19"/>
+    <mergeCell ref="D6:D19"/>
+    <mergeCell ref="F6:F19"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="E31:E36"/>
+    <mergeCell ref="G31:G36"/>
     <mergeCell ref="G6:G19"/>
     <mergeCell ref="C62:C76"/>
     <mergeCell ref="B62:B76"/>
@@ -2899,24 +2916,20 @@
     <mergeCell ref="D39:D42"/>
     <mergeCell ref="F39:F42"/>
     <mergeCell ref="G39:G42"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="E31:E36"/>
-    <mergeCell ref="G31:G36"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="B6:B19"/>
-    <mergeCell ref="C6:C19"/>
-    <mergeCell ref="D6:D19"/>
-    <mergeCell ref="F6:F19"/>
+    <mergeCell ref="B78:B83"/>
+    <mergeCell ref="C78:C83"/>
+    <mergeCell ref="D78:D83"/>
+    <mergeCell ref="F78:F83"/>
+    <mergeCell ref="G78:G83"/>
+    <mergeCell ref="B123:B127"/>
+    <mergeCell ref="C123:C127"/>
+    <mergeCell ref="D123:D127"/>
+    <mergeCell ref="G123:G127"/>
+    <mergeCell ref="B98:B103"/>
+    <mergeCell ref="C98:C103"/>
+    <mergeCell ref="D98:D103"/>
+    <mergeCell ref="F98:F103"/>
+    <mergeCell ref="G98:G103"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E22" location="Sheet1!C24" display="BaseNode" xr:uid="{9ABFF75D-D80B-4691-957A-F81DE47B1DCF}"/>

</xml_diff>